<commit_message>
feat: filter products by tag/category
</commit_message>
<xml_diff>
--- a/db/tables/products.xlsx
+++ b/db/tables/products.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
     <t xml:space="preserve">seller_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category_id</t>
   </si>
   <si>
     <t xml:space="preserve">Abraham</t>
@@ -358,10 +361,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31:B102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G104" activeCellId="0" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,813 +380,1119 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C22" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C24" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C26" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C27" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C29" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adding creating teable in faker
</commit_message>
<xml_diff>
--- a/db/tables/products.xlsx
+++ b/db/tables/products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">category_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
   </si>
   <si>
     <t xml:space="preserve">Abraham</t>
@@ -361,10 +364,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G104" activeCellId="0" sqref="G104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3:D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,10 +386,13 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -394,10 +400,13 @@
       <c r="C2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -405,10 +414,13 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -416,10 +428,13 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -427,10 +442,13 @@
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -438,10 +456,13 @@
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -449,10 +470,13 @@
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -460,10 +484,13 @@
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -471,10 +498,13 @@
       <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -482,10 +512,13 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -493,10 +526,13 @@
       <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -504,10 +540,13 @@
       <c r="C12" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
@@ -515,10 +554,13 @@
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -526,10 +568,13 @@
       <c r="C14" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -537,10 +582,13 @@
       <c r="C15" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -548,10 +596,13 @@
       <c r="C16" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>3</v>
@@ -559,10 +610,13 @@
       <c r="C17" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>3</v>
@@ -570,10 +624,13 @@
       <c r="C18" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3</v>
@@ -581,10 +638,13 @@
       <c r="C19" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
@@ -592,10 +652,13 @@
       <c r="C20" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
@@ -603,10 +666,13 @@
       <c r="C21" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>3</v>
@@ -614,10 +680,13 @@
       <c r="C22" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>3</v>
@@ -625,10 +694,13 @@
       <c r="C23" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
@@ -636,10 +708,13 @@
       <c r="C24" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>3</v>
@@ -647,10 +722,13 @@
       <c r="C25" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D25" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>3</v>
@@ -658,10 +736,13 @@
       <c r="C26" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>3</v>
@@ -669,10 +750,13 @@
       <c r="C27" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>3</v>
@@ -680,10 +764,13 @@
       <c r="C28" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>3</v>
@@ -691,808 +778,1030 @@
       <c r="C29" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C98" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C100" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>24</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>